<commit_message>
added conditional formatting to highlight location of price
</commit_message>
<xml_diff>
--- a/Price Lookup.xlsx
+++ b/Price Lookup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wasim\Desktop\Excel\Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{BE53A51A-A025-47F7-835D-843CF4C51E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68650F15-3A8D-4E72-987E-A1A8672279EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="3930" windowWidth="16455" windowHeight="11265"/>
+    <workbookView xWindow="525" yWindow="3255" windowWidth="23850" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Laptop</t>
   </si>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -165,11 +165,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -178,7 +177,15 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -487,11 +494,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +533,7 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>1000</v>
       </c>
       <c r="C2" s="2">
@@ -648,30 +655,39 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="6">
+      <c r="B12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="5">
         <f>IFERROR(INDEX(B2:F6,MATCH(B12,A2:A6,0),MATCH(C12,B1:F1,0)),0)</f>
-        <v>0</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:F7">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>B2=$D$12</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$2:$A$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>$B$1:$F$1</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>